<commit_message>
download upload, cleanup, metrics on smae line
</commit_message>
<xml_diff>
--- a/market_returns.xlsx
+++ b/market_returns.xlsx
@@ -1,22 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s0379635/SantanuBiswas/Personal/code/Streamlit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{08A1B0DF-96C7-C94E-B539-7B1449A079D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F67DE2C-86AC-9147-BA8A-882388ABAD1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17420" xr2:uid="{DEB3A457-C647-8A48-A70A-70538EAB9DCF}"/>
+    <workbookView xWindow="1100" yWindow="800" windowWidth="28040" windowHeight="17420" activeTab="3" xr2:uid="{DEB3A457-C647-8A48-A70A-70538EAB9DCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sim Data " sheetId="1" r:id="rId1"/>
     <sheet name="Raw Data" sheetId="2" r:id="rId2"/>
+    <sheet name="Correct Data" sheetId="4" r:id="rId3"/>
+    <sheet name="Statistics" sheetId="5" r:id="rId4"/>
+    <sheet name="Stats" sheetId="3" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">'Correct Data'!$B$1</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Correct Data'!$B$2:$B$100</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="15">
   <si>
     <t>Year</t>
   </si>
@@ -59,6 +66,30 @@
   <si>
     <t xml:space="preserve">US Bond </t>
   </si>
+  <si>
+    <t>Total Return</t>
+  </si>
+  <si>
+    <t>SKEW</t>
+  </si>
+  <si>
+    <t>KURT</t>
+  </si>
+  <si>
+    <t>MEAN</t>
+  </si>
+  <si>
+    <t>MEDIAN</t>
+  </si>
+  <si>
+    <t>STD DEV</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last 25 </t>
+  </si>
 </sst>
 </file>
 
@@ -67,7 +98,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -81,6 +112,41 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF373A3C"/>
+      <name val="Open Sans"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF373A3C"/>
+      <name val="Open Sans"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Open Sans"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF373A3C"/>
+      <name val="Open Sans"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF373A3C"/>
+      <name val="Open Sans"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Open Sans"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -104,7 +170,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -112,6 +178,14 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -128,6 +202,623 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.1</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>S&amp;P 500 Return - Histogram (1927 - 2024)</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="2000" b="1"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+            </a:rPr>
+            <a:t>S&amp;P 500 Return - Histogram (1927 - 2024)</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="clusteredColumn" uniqueId="{F9FDEEA6-8B5D-9948-A2A8-883F7258763F}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.0</cx:f>
+              <cx:v>Total Return</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:binning intervalClosed="r">
+              <cx:binSize val="4"/>
+            </cx:binning>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="0"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -220,6 +911,387 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="3" name="Chart 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63447A30-4596-F1D4-9F05-7EB593CA5B29}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8216900" y="584200"/>
+              <a:ext cx="10896600" cy="7226300"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1370119" cy="843501"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6ACBB8C-AAF8-C207-755F-1FD456774899}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4051300" y="990600"/>
+          <a:ext cx="1370119" cy="843501"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>Mean:  12.29</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>Median: 15.06</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>Std Dev: 19.57</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Straight Connector 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25F8FABD-5EA0-2790-C090-C42B916DC303}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7429500" y="2730500"/>
+          <a:ext cx="0" cy="4191000"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="31750">
+          <a:solidFill>
+            <a:srgbClr val="92D050"/>
+          </a:solidFill>
+          <a:prstDash val="sysDash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>197767</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="497765" cy="461665"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="TextBox 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD0913BD-5C44-BC48-E6E1-DE23E912BA0C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7188200" y="2991767"/>
+          <a:ext cx="497765" cy="461665"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="vert270" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" b="1"/>
+            <a:t>0 %</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Straight Connector 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82CBA83A-1009-644F-9351-D8CD9009E068}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="8712200" y="1663700"/>
+          <a:ext cx="0" cy="5245100"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="31750">
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+          <a:prstDash val="sysDash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>723901</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>121567</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="368300" cy="945233"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="TextBox 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B72693C-41A3-5547-BB1D-17F7417026AF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8445501" y="1899567"/>
+          <a:ext cx="368300" cy="945233"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" vert="vert270" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" b="1"/>
+            <a:t>Mean</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -542,8 +1614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35A51237-5C92-BF4C-8876-804CB8581436}">
   <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="O38" sqref="O38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2260,8 +3332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72764C98-6D09-DF4F-A0FB-81EC76BBE573}">
   <dimension ref="A1:E98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E1048576"/>
+    <sheetView topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3666,4 +4738,2833 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53AF4DDD-5653-A44C-8BB8-2CBF51826840}">
+  <dimension ref="A1:B104"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="32.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>2024</v>
+      </c>
+      <c r="B2" s="4">
+        <v>25.02</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2023</v>
+      </c>
+      <c r="B3" s="4">
+        <v>26.29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>2022</v>
+      </c>
+      <c r="B4" s="5">
+        <v>-18.11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>2021</v>
+      </c>
+      <c r="B5" s="4">
+        <v>28.71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>2020</v>
+      </c>
+      <c r="B6" s="4">
+        <v>18.399999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>2019</v>
+      </c>
+      <c r="B7" s="4">
+        <v>31.49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>2018</v>
+      </c>
+      <c r="B8" s="5">
+        <v>-4.38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>2017</v>
+      </c>
+      <c r="B9" s="4">
+        <v>21.83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>2016</v>
+      </c>
+      <c r="B10" s="4">
+        <v>11.96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>2015</v>
+      </c>
+      <c r="B11" s="4">
+        <v>1.38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>2014</v>
+      </c>
+      <c r="B12" s="4">
+        <v>13.69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>2013</v>
+      </c>
+      <c r="B13" s="4">
+        <v>32.39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>2012</v>
+      </c>
+      <c r="B14" s="4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>2011</v>
+      </c>
+      <c r="B15" s="4">
+        <v>2.11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>2010</v>
+      </c>
+      <c r="B16" s="4">
+        <v>15.06</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>2009</v>
+      </c>
+      <c r="B17" s="4">
+        <v>26.46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>2008</v>
+      </c>
+      <c r="B18" s="5">
+        <v>-37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>2007</v>
+      </c>
+      <c r="B19" s="4">
+        <v>5.49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>2006</v>
+      </c>
+      <c r="B20" s="4">
+        <v>15.79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>2005</v>
+      </c>
+      <c r="B21" s="4">
+        <v>4.91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>2004</v>
+      </c>
+      <c r="B22" s="4">
+        <v>10.88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>2003</v>
+      </c>
+      <c r="B23" s="4">
+        <v>28.68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>2002</v>
+      </c>
+      <c r="B24" s="5">
+        <v>-22.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>2001</v>
+      </c>
+      <c r="B25" s="5">
+        <v>-11.89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>2000</v>
+      </c>
+      <c r="B26" s="5">
+        <v>-9.1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>1999</v>
+      </c>
+      <c r="B27" s="4">
+        <v>21.04</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>1998</v>
+      </c>
+      <c r="B28" s="4">
+        <v>28.58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>1997</v>
+      </c>
+      <c r="B29" s="4">
+        <v>33.36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>1996</v>
+      </c>
+      <c r="B30" s="4">
+        <v>22.96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>1995</v>
+      </c>
+      <c r="B31" s="4">
+        <v>37.58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <v>1994</v>
+      </c>
+      <c r="B32" s="4">
+        <v>1.32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>1993</v>
+      </c>
+      <c r="B33" s="4">
+        <v>10.08</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>1992</v>
+      </c>
+      <c r="B34" s="4">
+        <v>7.62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <v>1991</v>
+      </c>
+      <c r="B35" s="4">
+        <v>30.47</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>1990</v>
+      </c>
+      <c r="B36" s="5">
+        <v>-3.1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <v>1989</v>
+      </c>
+      <c r="B37" s="4">
+        <v>31.69</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
+        <v>1988</v>
+      </c>
+      <c r="B38" s="4">
+        <v>16.61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
+        <v>1987</v>
+      </c>
+      <c r="B39" s="4">
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
+        <v>1986</v>
+      </c>
+      <c r="B40" s="4">
+        <v>18.670000000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A41" s="4">
+        <v>1985</v>
+      </c>
+      <c r="B41" s="4">
+        <v>31.73</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A42" s="4">
+        <v>1984</v>
+      </c>
+      <c r="B42" s="4">
+        <v>6.27</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A43" s="4">
+        <v>1983</v>
+      </c>
+      <c r="B43" s="4">
+        <v>22.56</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A44" s="4">
+        <v>1982</v>
+      </c>
+      <c r="B44" s="4">
+        <v>21.55</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A45" s="4">
+        <v>1981</v>
+      </c>
+      <c r="B45" s="5">
+        <v>-4.91</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A46" s="4">
+        <v>1980</v>
+      </c>
+      <c r="B46" s="4">
+        <v>32.42</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A47" s="4">
+        <v>1979</v>
+      </c>
+      <c r="B47" s="4">
+        <v>18.440000000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A48" s="4">
+        <v>1978</v>
+      </c>
+      <c r="B48" s="4">
+        <v>6.56</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A49" s="4">
+        <v>1977</v>
+      </c>
+      <c r="B49" s="5">
+        <v>-7.18</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A50" s="4">
+        <v>1976</v>
+      </c>
+      <c r="B50" s="4">
+        <v>23.84</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A51" s="4">
+        <v>1975</v>
+      </c>
+      <c r="B51" s="4">
+        <v>37.200000000000003</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A52" s="4">
+        <v>1974</v>
+      </c>
+      <c r="B52" s="5">
+        <v>-26.47</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A53" s="4">
+        <v>1973</v>
+      </c>
+      <c r="B53" s="5">
+        <v>-14.66</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A54" s="4">
+        <v>1972</v>
+      </c>
+      <c r="B54" s="4">
+        <v>18.98</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A55" s="4">
+        <v>1971</v>
+      </c>
+      <c r="B55" s="4">
+        <v>14.31</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A56" s="4">
+        <v>1970</v>
+      </c>
+      <c r="B56" s="4">
+        <v>4.01</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A57" s="4">
+        <v>1969</v>
+      </c>
+      <c r="B57" s="5">
+        <v>-8.5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A58" s="4">
+        <v>1968</v>
+      </c>
+      <c r="B58" s="4">
+        <v>11.06</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A59" s="4">
+        <v>1967</v>
+      </c>
+      <c r="B59" s="4">
+        <v>23.98</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A60" s="4">
+        <v>1966</v>
+      </c>
+      <c r="B60" s="5">
+        <v>-10.06</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A61" s="4">
+        <v>1965</v>
+      </c>
+      <c r="B61" s="4">
+        <v>12.45</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A62" s="4">
+        <v>1964</v>
+      </c>
+      <c r="B62" s="4">
+        <v>16.48</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A63" s="4">
+        <v>1963</v>
+      </c>
+      <c r="B63" s="4">
+        <v>22.8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A64" s="4">
+        <v>1962</v>
+      </c>
+      <c r="B64" s="5">
+        <v>-8.73</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A65" s="4">
+        <v>1961</v>
+      </c>
+      <c r="B65" s="4">
+        <v>26.89</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A66" s="4">
+        <v>1960</v>
+      </c>
+      <c r="B66" s="4">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A67" s="4">
+        <v>1959</v>
+      </c>
+      <c r="B67" s="4">
+        <v>11.96</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A68" s="4">
+        <v>1958</v>
+      </c>
+      <c r="B68" s="4">
+        <v>43.36</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A69" s="4">
+        <v>1957</v>
+      </c>
+      <c r="B69" s="5">
+        <v>-10.78</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A70" s="4">
+        <v>1956</v>
+      </c>
+      <c r="B70" s="4">
+        <v>6.56</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A71" s="4">
+        <v>1955</v>
+      </c>
+      <c r="B71" s="4">
+        <v>31.56</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A72" s="4">
+        <v>1954</v>
+      </c>
+      <c r="B72" s="4">
+        <v>52.62</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A73" s="4">
+        <v>1953</v>
+      </c>
+      <c r="B73" s="5">
+        <v>-0.99</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A74" s="4">
+        <v>1952</v>
+      </c>
+      <c r="B74" s="4">
+        <v>18.37</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A75" s="4">
+        <v>1951</v>
+      </c>
+      <c r="B75" s="4">
+        <v>24.02</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A76" s="4">
+        <v>1950</v>
+      </c>
+      <c r="B76" s="4">
+        <v>31.71</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A77" s="4">
+        <v>1949</v>
+      </c>
+      <c r="B77" s="4">
+        <v>18.79</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A78" s="4">
+        <v>1948</v>
+      </c>
+      <c r="B78" s="4">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A79" s="4">
+        <v>1947</v>
+      </c>
+      <c r="B79" s="4">
+        <v>5.71</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A80" s="4">
+        <v>1946</v>
+      </c>
+      <c r="B80" s="5">
+        <v>-8.07</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A81" s="4">
+        <v>1945</v>
+      </c>
+      <c r="B81" s="4">
+        <v>36.44</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A82" s="4">
+        <v>1944</v>
+      </c>
+      <c r="B82" s="4">
+        <v>19.75</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A83" s="4">
+        <v>1943</v>
+      </c>
+      <c r="B83" s="4">
+        <v>25.9</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A84" s="4">
+        <v>1942</v>
+      </c>
+      <c r="B84" s="4">
+        <v>20.34</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A85" s="4">
+        <v>1941</v>
+      </c>
+      <c r="B85" s="5">
+        <v>-11.59</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A86" s="4">
+        <v>1940</v>
+      </c>
+      <c r="B86" s="5">
+        <v>-9.7799999999999994</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A87" s="4">
+        <v>1939</v>
+      </c>
+      <c r="B87" s="5">
+        <v>-0.41</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A88" s="4">
+        <v>1938</v>
+      </c>
+      <c r="B88" s="4">
+        <v>31.12</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A89" s="4">
+        <v>1937</v>
+      </c>
+      <c r="B89" s="5">
+        <v>-35.03</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A90" s="4">
+        <v>1936</v>
+      </c>
+      <c r="B90" s="4">
+        <v>33.92</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A91" s="4">
+        <v>1935</v>
+      </c>
+      <c r="B91" s="4">
+        <v>47.67</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A92" s="4">
+        <v>1934</v>
+      </c>
+      <c r="B92" s="5">
+        <v>-1.44</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A93" s="4">
+        <v>1933</v>
+      </c>
+      <c r="B93" s="4">
+        <v>53.99</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A94" s="4">
+        <v>1932</v>
+      </c>
+      <c r="B94" s="5">
+        <v>-8.19</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A95" s="4">
+        <v>1931</v>
+      </c>
+      <c r="B95" s="5">
+        <v>-43.34</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A96" s="4">
+        <v>1930</v>
+      </c>
+      <c r="B96" s="5">
+        <v>-24.9</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A97" s="4">
+        <v>1929</v>
+      </c>
+      <c r="B97" s="5">
+        <v>-8.42</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A98" s="4">
+        <v>1928</v>
+      </c>
+      <c r="B98" s="4">
+        <v>43.61</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A99" s="4">
+        <v>1927</v>
+      </c>
+      <c r="B99" s="4">
+        <v>37.49</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A100" s="4">
+        <v>1926</v>
+      </c>
+      <c r="B100" s="4">
+        <v>11.62</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B102" s="6">
+        <f>MEDIAN(B2:B100)</f>
+        <v>15.06</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B103" s="6">
+        <f>AVERAGE(B2:B100)</f>
+        <v>12.289393939393936</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B104" s="6">
+        <f>_xlfn.STDEV.P(B2:B100)</f>
+        <v>19.565181700823178</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E98E660-7BF1-C74A-B8ED-7DA7266A7B57}">
+  <dimension ref="A1:H100"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="13" style="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="20" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="20" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
+        <v>1926</v>
+      </c>
+      <c r="B2" s="8">
+        <v>11.62</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="10">
+        <f>SKEW(B2:B100)</f>
+        <v>-0.4362342014609345</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="10">
+        <f>SKEW(B76:B100)</f>
+        <v>-0.86504028529909949</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="20" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
+        <v>1927</v>
+      </c>
+      <c r="B3" s="8">
+        <v>37.49</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="10">
+        <f>KURT(B2:B100)</f>
+        <v>5.568074672609491E-2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="10">
+        <f>KURT(B2:B100)</f>
+        <v>5.568074672609491E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="20" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>1928</v>
+      </c>
+      <c r="B4" s="8">
+        <v>43.61</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="10">
+        <f>AVERAGE(B2:B100)</f>
+        <v>12.289393939393943</v>
+      </c>
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="10">
+        <f>AVERAGE(B76:B100)</f>
+        <v>9.3584000000000014</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="20" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>1929</v>
+      </c>
+      <c r="B5" s="9">
+        <v>-8.42</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="10">
+        <f>MEDIAN(B2:B100)</f>
+        <v>15.06</v>
+      </c>
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="10">
+        <f>MEDIAN(B76:B100)</f>
+        <v>13.69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="20" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>1930</v>
+      </c>
+      <c r="B6" s="9">
+        <v>-24.9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="10">
+        <f>STDEV(B2:B100)</f>
+        <v>19.664750698574988</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="10">
+        <f>STDEV(B76:B100)</f>
+        <v>18.258292107058281</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="20" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>1931</v>
+      </c>
+      <c r="B7" s="9">
+        <v>-43.34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="20" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>1932</v>
+      </c>
+      <c r="B8" s="9">
+        <v>-8.19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="20" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>1933</v>
+      </c>
+      <c r="B9" s="8">
+        <v>53.99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="20" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <v>1934</v>
+      </c>
+      <c r="B10" s="9">
+        <v>-1.44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="20" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
+        <v>1935</v>
+      </c>
+      <c r="B11" s="8">
+        <v>47.67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="20" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
+        <v>1936</v>
+      </c>
+      <c r="B12" s="8">
+        <v>33.92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="20" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
+        <v>1937</v>
+      </c>
+      <c r="B13" s="9">
+        <v>-35.03</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="20" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
+        <v>1938</v>
+      </c>
+      <c r="B14" s="8">
+        <v>31.12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="20" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
+        <v>1939</v>
+      </c>
+      <c r="B15" s="9">
+        <v>-0.41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="20" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
+        <v>1940</v>
+      </c>
+      <c r="B16" s="9">
+        <v>-9.7799999999999994</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
+        <v>1941</v>
+      </c>
+      <c r="B17" s="9">
+        <v>-11.59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
+        <v>1942</v>
+      </c>
+      <c r="B18" s="8">
+        <v>20.34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
+        <v>1943</v>
+      </c>
+      <c r="B19" s="8">
+        <v>25.9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
+        <v>1944</v>
+      </c>
+      <c r="B20" s="8">
+        <v>19.75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A21" s="8">
+        <v>1945</v>
+      </c>
+      <c r="B21" s="8">
+        <v>36.44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A22" s="8">
+        <v>1946</v>
+      </c>
+      <c r="B22" s="9">
+        <v>-8.07</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A23" s="8">
+        <v>1947</v>
+      </c>
+      <c r="B23" s="8">
+        <v>5.71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A24" s="8">
+        <v>1948</v>
+      </c>
+      <c r="B24" s="8">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A25" s="8">
+        <v>1949</v>
+      </c>
+      <c r="B25" s="8">
+        <v>18.79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A26" s="8">
+        <v>1950</v>
+      </c>
+      <c r="B26" s="8">
+        <v>31.71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A27" s="8">
+        <v>1951</v>
+      </c>
+      <c r="B27" s="8">
+        <v>24.02</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A28" s="8">
+        <v>1952</v>
+      </c>
+      <c r="B28" s="8">
+        <v>18.37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A29" s="8">
+        <v>1953</v>
+      </c>
+      <c r="B29" s="9">
+        <v>-0.99</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A30" s="8">
+        <v>1954</v>
+      </c>
+      <c r="B30" s="8">
+        <v>52.62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A31" s="8">
+        <v>1955</v>
+      </c>
+      <c r="B31" s="8">
+        <v>31.56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A32" s="8">
+        <v>1956</v>
+      </c>
+      <c r="B32" s="8">
+        <v>6.56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A33" s="8">
+        <v>1957</v>
+      </c>
+      <c r="B33" s="9">
+        <v>-10.78</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A34" s="8">
+        <v>1958</v>
+      </c>
+      <c r="B34" s="8">
+        <v>43.36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A35" s="8">
+        <v>1959</v>
+      </c>
+      <c r="B35" s="8">
+        <v>11.96</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A36" s="8">
+        <v>1960</v>
+      </c>
+      <c r="B36" s="8">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A37" s="8">
+        <v>1961</v>
+      </c>
+      <c r="B37" s="8">
+        <v>26.89</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A38" s="8">
+        <v>1962</v>
+      </c>
+      <c r="B38" s="9">
+        <v>-8.73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A39" s="8">
+        <v>1963</v>
+      </c>
+      <c r="B39" s="8">
+        <v>22.8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A40" s="8">
+        <v>1964</v>
+      </c>
+      <c r="B40" s="8">
+        <v>16.48</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A41" s="8">
+        <v>1965</v>
+      </c>
+      <c r="B41" s="8">
+        <v>12.45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A42" s="8">
+        <v>1966</v>
+      </c>
+      <c r="B42" s="9">
+        <v>-10.06</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A43" s="8">
+        <v>1967</v>
+      </c>
+      <c r="B43" s="8">
+        <v>23.98</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A44" s="8">
+        <v>1968</v>
+      </c>
+      <c r="B44" s="8">
+        <v>11.06</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A45" s="8">
+        <v>1969</v>
+      </c>
+      <c r="B45" s="9">
+        <v>-8.5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A46" s="8">
+        <v>1970</v>
+      </c>
+      <c r="B46" s="8">
+        <v>4.01</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A47" s="8">
+        <v>1971</v>
+      </c>
+      <c r="B47" s="8">
+        <v>14.31</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A48" s="8">
+        <v>1972</v>
+      </c>
+      <c r="B48" s="8">
+        <v>18.98</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A49" s="8">
+        <v>1973</v>
+      </c>
+      <c r="B49" s="9">
+        <v>-14.66</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A50" s="8">
+        <v>1974</v>
+      </c>
+      <c r="B50" s="9">
+        <v>-26.47</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A51" s="8">
+        <v>1975</v>
+      </c>
+      <c r="B51" s="8">
+        <v>37.200000000000003</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A52" s="8">
+        <v>1976</v>
+      </c>
+      <c r="B52" s="8">
+        <v>23.84</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A53" s="8">
+        <v>1977</v>
+      </c>
+      <c r="B53" s="9">
+        <v>-7.18</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A54" s="8">
+        <v>1978</v>
+      </c>
+      <c r="B54" s="8">
+        <v>6.56</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A55" s="8">
+        <v>1979</v>
+      </c>
+      <c r="B55" s="8">
+        <v>18.440000000000001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A56" s="8">
+        <v>1980</v>
+      </c>
+      <c r="B56" s="8">
+        <v>32.42</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A57" s="8">
+        <v>1981</v>
+      </c>
+      <c r="B57" s="9">
+        <v>-4.91</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A58" s="8">
+        <v>1982</v>
+      </c>
+      <c r="B58" s="8">
+        <v>21.55</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A59" s="8">
+        <v>1983</v>
+      </c>
+      <c r="B59" s="8">
+        <v>22.56</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A60" s="8">
+        <v>1984</v>
+      </c>
+      <c r="B60" s="8">
+        <v>6.27</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A61" s="8">
+        <v>1985</v>
+      </c>
+      <c r="B61" s="8">
+        <v>31.73</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A62" s="8">
+        <v>1986</v>
+      </c>
+      <c r="B62" s="8">
+        <v>18.670000000000002</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A63" s="8">
+        <v>1987</v>
+      </c>
+      <c r="B63" s="8">
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A64" s="8">
+        <v>1988</v>
+      </c>
+      <c r="B64" s="8">
+        <v>16.61</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A65" s="8">
+        <v>1989</v>
+      </c>
+      <c r="B65" s="8">
+        <v>31.69</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A66" s="8">
+        <v>1990</v>
+      </c>
+      <c r="B66" s="9">
+        <v>-3.1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A67" s="8">
+        <v>1991</v>
+      </c>
+      <c r="B67" s="8">
+        <v>30.47</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A68" s="8">
+        <v>1992</v>
+      </c>
+      <c r="B68" s="8">
+        <v>7.62</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A69" s="8">
+        <v>1993</v>
+      </c>
+      <c r="B69" s="8">
+        <v>10.08</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A70" s="8">
+        <v>1994</v>
+      </c>
+      <c r="B70" s="8">
+        <v>1.32</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A71" s="8">
+        <v>1995</v>
+      </c>
+      <c r="B71" s="8">
+        <v>37.58</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A72" s="8">
+        <v>1996</v>
+      </c>
+      <c r="B72" s="8">
+        <v>22.96</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A73" s="8">
+        <v>1997</v>
+      </c>
+      <c r="B73" s="8">
+        <v>33.36</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A74" s="8">
+        <v>1998</v>
+      </c>
+      <c r="B74" s="8">
+        <v>28.58</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A75" s="8">
+        <v>1999</v>
+      </c>
+      <c r="B75" s="8">
+        <v>21.04</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A76" s="8">
+        <v>2000</v>
+      </c>
+      <c r="B76" s="9">
+        <v>-9.1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A77" s="8">
+        <v>2001</v>
+      </c>
+      <c r="B77" s="9">
+        <v>-11.89</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A78" s="8">
+        <v>2002</v>
+      </c>
+      <c r="B78" s="9">
+        <v>-22.1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A79" s="8">
+        <v>2003</v>
+      </c>
+      <c r="B79" s="8">
+        <v>28.68</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A80" s="8">
+        <v>2004</v>
+      </c>
+      <c r="B80" s="8">
+        <v>10.88</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A81" s="8">
+        <v>2005</v>
+      </c>
+      <c r="B81" s="8">
+        <v>4.91</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A82" s="8">
+        <v>2006</v>
+      </c>
+      <c r="B82" s="8">
+        <v>15.79</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A83" s="8">
+        <v>2007</v>
+      </c>
+      <c r="B83" s="8">
+        <v>5.49</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A84" s="8">
+        <v>2008</v>
+      </c>
+      <c r="B84" s="9">
+        <v>-37</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A85" s="8">
+        <v>2009</v>
+      </c>
+      <c r="B85" s="8">
+        <v>26.46</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A86" s="8">
+        <v>2010</v>
+      </c>
+      <c r="B86" s="8">
+        <v>15.06</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A87" s="8">
+        <v>2011</v>
+      </c>
+      <c r="B87" s="8">
+        <v>2.11</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A88" s="8">
+        <v>2012</v>
+      </c>
+      <c r="B88" s="8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A89" s="8">
+        <v>2013</v>
+      </c>
+      <c r="B89" s="8">
+        <v>32.39</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A90" s="8">
+        <v>2014</v>
+      </c>
+      <c r="B90" s="8">
+        <v>13.69</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A91" s="8">
+        <v>2015</v>
+      </c>
+      <c r="B91" s="8">
+        <v>1.38</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A92" s="8">
+        <v>2016</v>
+      </c>
+      <c r="B92" s="8">
+        <v>11.96</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A93" s="8">
+        <v>2017</v>
+      </c>
+      <c r="B93" s="8">
+        <v>21.83</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A94" s="8">
+        <v>2018</v>
+      </c>
+      <c r="B94" s="9">
+        <v>-4.38</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A95" s="8">
+        <v>2019</v>
+      </c>
+      <c r="B95" s="8">
+        <v>31.49</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A96" s="8">
+        <v>2020</v>
+      </c>
+      <c r="B96" s="8">
+        <v>18.399999999999999</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A97" s="8">
+        <v>2021</v>
+      </c>
+      <c r="B97" s="8">
+        <v>28.71</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A98" s="8">
+        <v>2022</v>
+      </c>
+      <c r="B98" s="9">
+        <v>-18.11</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A99" s="8">
+        <v>2023</v>
+      </c>
+      <c r="B99" s="8">
+        <v>26.29</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A100" s="8">
+        <v>2024</v>
+      </c>
+      <c r="B100" s="8">
+        <v>25.02</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B100">
+    <sortCondition ref="A2:A100"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{293A1855-2E61-1D44-8FB7-9F3A7378979B}">
+  <dimension ref="A1:C98"/>
+  <sheetViews>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1927</v>
+      </c>
+      <c r="B2" s="1">
+        <v>37.49</v>
+      </c>
+      <c r="C2" s="1">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>1928</v>
+      </c>
+      <c r="B3" s="1">
+        <v>43.61</v>
+      </c>
+      <c r="C3" s="1">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>1929</v>
+      </c>
+      <c r="B4" s="1">
+        <v>-8.3000000000000007</v>
+      </c>
+      <c r="C4" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>1930</v>
+      </c>
+      <c r="B5" s="1">
+        <v>-24.9</v>
+      </c>
+      <c r="C5" s="1">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>1931</v>
+      </c>
+      <c r="B6" s="1">
+        <v>-43.34</v>
+      </c>
+      <c r="C6" s="1">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>1932</v>
+      </c>
+      <c r="B7" s="1">
+        <v>-8.19</v>
+      </c>
+      <c r="C7" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>1933</v>
+      </c>
+      <c r="B8" s="1">
+        <v>53.99</v>
+      </c>
+      <c r="C8" s="1">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>1934</v>
+      </c>
+      <c r="B9" s="1">
+        <v>-1.44</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>1935</v>
+      </c>
+      <c r="B10" s="1">
+        <v>47.67</v>
+      </c>
+      <c r="C10" s="1">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>1936</v>
+      </c>
+      <c r="B11" s="1">
+        <v>-10.46</v>
+      </c>
+      <c r="C11" s="1">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>1937</v>
+      </c>
+      <c r="B12" s="1">
+        <v>-33.799999999999997</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>1938</v>
+      </c>
+      <c r="B13" s="1">
+        <v>-35.03</v>
+      </c>
+      <c r="C13" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>1939</v>
+      </c>
+      <c r="B14" s="1">
+        <v>-26.47</v>
+      </c>
+      <c r="C14" s="1">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>1940</v>
+      </c>
+      <c r="B15" s="1">
+        <v>-11.59</v>
+      </c>
+      <c r="C15" s="1">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>1941</v>
+      </c>
+      <c r="B16" s="1">
+        <v>-10.119999999999999</v>
+      </c>
+      <c r="C16" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>1942</v>
+      </c>
+      <c r="B17" s="1">
+        <v>-8.19</v>
+      </c>
+      <c r="C17" s="1">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>1943</v>
+      </c>
+      <c r="B18" s="1">
+        <v>23.13</v>
+      </c>
+      <c r="C18" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>1944</v>
+      </c>
+      <c r="B19" s="1">
+        <v>19.45</v>
+      </c>
+      <c r="C19" s="1">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>1945</v>
+      </c>
+      <c r="B20" s="1">
+        <v>35.82</v>
+      </c>
+      <c r="C20" s="1">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>1946</v>
+      </c>
+      <c r="B21" s="1">
+        <v>24.02</v>
+      </c>
+      <c r="C21" s="1">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>1947</v>
+      </c>
+      <c r="B22" s="1">
+        <v>5.71</v>
+      </c>
+      <c r="C22" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>1948</v>
+      </c>
+      <c r="B23" s="1">
+        <v>18.8</v>
+      </c>
+      <c r="C23" s="1">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>1949</v>
+      </c>
+      <c r="B24" s="1">
+        <v>31.71</v>
+      </c>
+      <c r="C24" s="1">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>1950</v>
+      </c>
+      <c r="B25" s="1">
+        <v>-0.92</v>
+      </c>
+      <c r="C25" s="1">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>1951</v>
+      </c>
+      <c r="B26" s="1">
+        <v>-10.5</v>
+      </c>
+      <c r="C26" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>1952</v>
+      </c>
+      <c r="B27" s="1">
+        <v>20.43</v>
+      </c>
+      <c r="C27" s="1">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>1953</v>
+      </c>
+      <c r="B28" s="1">
+        <v>36.28</v>
+      </c>
+      <c r="C28" s="1">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>1954</v>
+      </c>
+      <c r="B29" s="1">
+        <v>24.43</v>
+      </c>
+      <c r="C29" s="1">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>1955</v>
+      </c>
+      <c r="B30" s="1">
+        <v>2.62</v>
+      </c>
+      <c r="C30" s="1">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>1956</v>
+      </c>
+      <c r="B31" s="1">
+        <v>16.41</v>
+      </c>
+      <c r="C31" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>1957</v>
+      </c>
+      <c r="B32" s="1">
+        <v>12.06</v>
+      </c>
+      <c r="C32" s="1">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>1958</v>
+      </c>
+      <c r="B33" s="1">
+        <v>0.47</v>
+      </c>
+      <c r="C33" s="1">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>1959</v>
+      </c>
+      <c r="B34" s="1">
+        <v>23.13</v>
+      </c>
+      <c r="C34" s="1">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>1960</v>
+      </c>
+      <c r="B35" s="1">
+        <v>8.99</v>
+      </c>
+      <c r="C35" s="1">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>1961</v>
+      </c>
+      <c r="B36" s="1">
+        <v>-1.95</v>
+      </c>
+      <c r="C36" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>1962</v>
+      </c>
+      <c r="B37" s="1">
+        <v>13.48</v>
+      </c>
+      <c r="C37" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>1963</v>
+      </c>
+      <c r="B38" s="1">
+        <v>19.149999999999999</v>
+      </c>
+      <c r="C38" s="1">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>1964</v>
+      </c>
+      <c r="B39" s="1">
+        <v>32.42</v>
+      </c>
+      <c r="C39" s="1">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>1965</v>
+      </c>
+      <c r="B40" s="1">
+        <v>6.56</v>
+      </c>
+      <c r="C40" s="1">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>1966</v>
+      </c>
+      <c r="B41" s="1">
+        <v>18.440000000000001</v>
+      </c>
+      <c r="C41" s="1">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>1967</v>
+      </c>
+      <c r="B42" s="1">
+        <v>31.55</v>
+      </c>
+      <c r="C42" s="1">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>1968</v>
+      </c>
+      <c r="B43" s="1">
+        <v>18.61</v>
+      </c>
+      <c r="C43" s="1">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>1969</v>
+      </c>
+      <c r="B44" s="1">
+        <v>5.23</v>
+      </c>
+      <c r="C44" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>1970</v>
+      </c>
+      <c r="B45" s="1">
+        <v>16.61</v>
+      </c>
+      <c r="C45" s="1">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <v>1971</v>
+      </c>
+      <c r="B46" s="1">
+        <v>31.73</v>
+      </c>
+      <c r="C46" s="1">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>1972</v>
+      </c>
+      <c r="B47" s="1">
+        <v>-3.06</v>
+      </c>
+      <c r="C47" s="1">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>1973</v>
+      </c>
+      <c r="B48" s="1">
+        <v>30.23</v>
+      </c>
+      <c r="C48" s="1">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>1974</v>
+      </c>
+      <c r="B49" s="1">
+        <v>7.62</v>
+      </c>
+      <c r="C49" s="1">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <v>1975</v>
+      </c>
+      <c r="B50" s="1">
+        <v>10.08</v>
+      </c>
+      <c r="C50" s="1">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>1976</v>
+      </c>
+      <c r="B51" s="1">
+        <v>1.32</v>
+      </c>
+      <c r="C51" s="1">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>1977</v>
+      </c>
+      <c r="B52" s="1">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="C52" s="1">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <v>1978</v>
+      </c>
+      <c r="B53" s="1">
+        <v>22.68</v>
+      </c>
+      <c r="C53" s="1">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>1979</v>
+      </c>
+      <c r="B54" s="1">
+        <v>33.36</v>
+      </c>
+      <c r="C54" s="1">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <v>1980</v>
+      </c>
+      <c r="B55" s="1">
+        <v>28.58</v>
+      </c>
+      <c r="C55" s="1">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <v>1981</v>
+      </c>
+      <c r="B56" s="1">
+        <v>21.55</v>
+      </c>
+      <c r="C56" s="1">
+        <v>4.8999999999999986</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <v>1982</v>
+      </c>
+      <c r="B57" s="1">
+        <v>-9.1</v>
+      </c>
+      <c r="C57" s="1">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <v>1983</v>
+      </c>
+      <c r="B58" s="1">
+        <v>-11.89</v>
+      </c>
+      <c r="C58" s="1">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <v>1984</v>
+      </c>
+      <c r="B59" s="1">
+        <v>-21.97</v>
+      </c>
+      <c r="C59" s="1">
+        <v>4.1000000000000014</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
+        <v>1985</v>
+      </c>
+      <c r="B60" s="1">
+        <v>28.36</v>
+      </c>
+      <c r="C60" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <v>1986</v>
+      </c>
+      <c r="B61" s="1">
+        <v>10.74</v>
+      </c>
+      <c r="C61" s="1">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <v>1987</v>
+      </c>
+      <c r="B62" s="1">
+        <v>5.33</v>
+      </c>
+      <c r="C62" s="1">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
+        <v>1988</v>
+      </c>
+      <c r="B63" s="1">
+        <v>15.11</v>
+      </c>
+      <c r="C63" s="1">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
+        <v>1989</v>
+      </c>
+      <c r="B64" s="1">
+        <v>5.98</v>
+      </c>
+      <c r="C64" s="1">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="1">
+        <v>1990</v>
+      </c>
+      <c r="B65" s="1">
+        <v>15.76</v>
+      </c>
+      <c r="C65" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
+        <v>1991</v>
+      </c>
+      <c r="B66" s="1">
+        <v>31.51</v>
+      </c>
+      <c r="C66" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="1">
+        <v>1992</v>
+      </c>
+      <c r="B67" s="1">
+        <v>18.170000000000002</v>
+      </c>
+      <c r="C67" s="1">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
+        <v>1993</v>
+      </c>
+      <c r="B68" s="1">
+        <v>5.99</v>
+      </c>
+      <c r="C68" s="1">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="1">
+        <v>1994</v>
+      </c>
+      <c r="B69" s="1">
+        <v>15.5</v>
+      </c>
+      <c r="C69" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="1">
+        <v>1995</v>
+      </c>
+      <c r="B70" s="1">
+        <v>32.89</v>
+      </c>
+      <c r="C70" s="1">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="1">
+        <v>1996</v>
+      </c>
+      <c r="B71" s="1">
+        <v>13.19</v>
+      </c>
+      <c r="C71" s="1">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="1">
+        <v>1997</v>
+      </c>
+      <c r="B72" s="1">
+        <v>1.88</v>
+      </c>
+      <c r="C72" s="1">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="1">
+        <v>1998</v>
+      </c>
+      <c r="B73" s="1">
+        <v>11.46</v>
+      </c>
+      <c r="C73" s="1">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="1">
+        <v>1999</v>
+      </c>
+      <c r="B74" s="1">
+        <v>-21.6</v>
+      </c>
+      <c r="C74" s="1">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="1">
+        <v>2000</v>
+      </c>
+      <c r="B75" s="1">
+        <v>28.18</v>
+      </c>
+      <c r="C75" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" s="1">
+        <v>2001</v>
+      </c>
+      <c r="B76" s="1">
+        <v>11.38</v>
+      </c>
+      <c r="C76" s="1">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="1">
+        <v>2002</v>
+      </c>
+      <c r="B77" s="1">
+        <v>4.41</v>
+      </c>
+      <c r="C77" s="1">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="1">
+        <v>2003</v>
+      </c>
+      <c r="B78" s="1">
+        <v>16.29</v>
+      </c>
+      <c r="C78" s="1">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="1">
+        <v>2004</v>
+      </c>
+      <c r="B79" s="1">
+        <v>4.99</v>
+      </c>
+      <c r="C79" s="1">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" s="1">
+        <v>2005</v>
+      </c>
+      <c r="B80" s="1">
+        <v>-36.5</v>
+      </c>
+      <c r="C80" s="1">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" s="1">
+        <v>2006</v>
+      </c>
+      <c r="B81" s="1">
+        <v>25.96</v>
+      </c>
+      <c r="C81" s="1">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" s="1">
+        <v>2007</v>
+      </c>
+      <c r="B82" s="1">
+        <v>15.56</v>
+      </c>
+      <c r="C82" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" s="1">
+        <v>2008</v>
+      </c>
+      <c r="B83" s="1">
+        <v>1.61</v>
+      </c>
+      <c r="C83" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" s="1">
+        <v>2009</v>
+      </c>
+      <c r="B84" s="1">
+        <v>16.5</v>
+      </c>
+      <c r="C84" s="1">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" s="1">
+        <v>2010</v>
+      </c>
+      <c r="B85" s="1">
+        <v>31.89</v>
+      </c>
+      <c r="C85" s="1">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" s="1">
+        <v>2011</v>
+      </c>
+      <c r="B86" s="1">
+        <v>14.19</v>
+      </c>
+      <c r="C86" s="1">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" s="1">
+        <v>2012</v>
+      </c>
+      <c r="B87" s="1">
+        <v>0.87999999999999989</v>
+      </c>
+      <c r="C87" s="1">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" s="1">
+        <v>2013</v>
+      </c>
+      <c r="B88" s="1">
+        <v>12.46</v>
+      </c>
+      <c r="C88" s="1">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B89" s="1">
+        <v>-22.6</v>
+      </c>
+      <c r="C89" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" s="1">
+        <v>2015</v>
+      </c>
+      <c r="B90" s="1">
+        <v>29.18</v>
+      </c>
+      <c r="C90" s="1">
+        <v>4.8999999999999986</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B91" s="1">
+        <v>10.38</v>
+      </c>
+      <c r="C91" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B92" s="1">
+        <v>5.41</v>
+      </c>
+      <c r="C92" s="1">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" s="1">
+        <v>2018</v>
+      </c>
+      <c r="B93" s="1">
+        <v>15.29</v>
+      </c>
+      <c r="C93" s="1">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" s="1">
+        <v>2019</v>
+      </c>
+      <c r="B94" s="1">
+        <v>5.99</v>
+      </c>
+      <c r="C94" s="1">
+        <v>5.8999999999999986</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" s="1">
+        <v>2020</v>
+      </c>
+      <c r="B95" s="1">
+        <v>-37.5</v>
+      </c>
+      <c r="C95" s="1">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" s="1">
+        <v>2021</v>
+      </c>
+      <c r="B96" s="1">
+        <v>26.96</v>
+      </c>
+      <c r="C96" s="1">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B97" s="1">
+        <v>14.56</v>
+      </c>
+      <c r="C97" s="1">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B98" s="1">
+        <v>2.61</v>
+      </c>
+      <c r="C98" s="1">
+        <v>6.6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>